<commit_message>
Update AI Capability Analysis
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/AI Capability Analysis.xlsx
+++ b/AI Capability Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9628cc1627804b4b/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9628cc1627804b4b/Development/AI Capability Map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F69A5E8-B208-4E44-81C9-CB0A553AA66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{3F69A5E8-B208-4E44-81C9-CB0A553AA66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2C84BD2-A5B3-F845-AB4E-C77DB1B9DD45}"/>
   <bookViews>
-    <workbookView xWindow="20700" yWindow="1725" windowWidth="29445" windowHeight="18435" xr2:uid="{DC6190FD-2F33-4231-8012-03A899A968AF}"/>
+    <workbookView xWindow="-33500" yWindow="-8220" windowWidth="27040" windowHeight="16860" activeTab="3" xr2:uid="{DC6190FD-2F33-4231-8012-03A899A968AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="9" r:id="rId1"/>
@@ -1817,7 +1817,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1839,9 +1839,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1868,6 +1865,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2205,35 +2208,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12A2F14-CAA6-4F55-9520-89D772075049}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" customWidth="1"/>
+    <col min="1" max="1" width="55.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="4" width="3.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>509</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="24" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <v>46013</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>502</v>
       </c>
@@ -2244,7 +2247,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>444</v>
       </c>
@@ -2267,9 +2270,9 @@
         <v>476</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="C7" s="10"/>
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="9"/>
+      <c r="C7" s="9"/>
       <c r="E7" s="6" t="s">
         <v>477</v>
       </c>
@@ -2286,11 +2289,11 @@
         <v>481</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>445</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>459</v>
       </c>
       <c r="E8" s="6" t="s">
@@ -2309,11 +2312,11 @@
         <v>485</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>446</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>460</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -2332,11 +2335,11 @@
         <v>485</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>461</v>
       </c>
       <c r="E10" s="6" t="s">
@@ -2355,11 +2358,11 @@
         <v>488</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>462</v>
       </c>
       <c r="E11" s="6" t="s">
@@ -2378,11 +2381,11 @@
         <v>490</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>463</v>
       </c>
       <c r="E12" s="6" t="s">
@@ -2401,11 +2404,11 @@
         <v>485</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>450</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>464</v>
       </c>
       <c r="E13" s="6" t="s">
@@ -2424,12 +2427,12 @@
         <v>488</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E14" s="1" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>503</v>
       </c>
@@ -2437,142 +2440,142 @@
         <v>465</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="C16" s="10"/>
+    <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A16" s="9"/>
+      <c r="C16" s="9"/>
       <c r="E16" s="7" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
         <v>451</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
         <v>452</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>467</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
         <v>453</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>468</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
         <v>454</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>469</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="12" t="s">
         <v>510</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
         <v>455</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>470</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="12" t="s">
         <v>493</v>
       </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="12" t="s">
         <v>494</v>
       </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
         <v>457</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="12" t="s">
         <v>495</v>
       </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E24" s="15" t="s">
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E24" s="14" t="s">
         <v>496</v>
       </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E25" s="15" t="s">
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E25" s="14" t="s">
         <v>497</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E26" s="15" t="s">
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E26" s="14" t="s">
         <v>498</v>
       </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E27" s="15" t="s">
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E27" s="14" t="s">
         <v>499</v>
       </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E29" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E30" s="13" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E30" s="12" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E31" s="13" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E31" s="12" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+    <row r="34" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="16"/>
+    </row>
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -2582,7 +2585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>0</v>
       </c>
@@ -2593,7 +2596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>1</v>
       </c>
@@ -2604,7 +2607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>2</v>
       </c>
@@ -2615,7 +2618,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>3</v>
       </c>
@@ -2626,7 +2629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>4</v>
       </c>
@@ -2637,7 +2640,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>5</v>
       </c>
@@ -2657,21 +2660,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C5AB6-1B90-4542-922B-2DF111E71EC5}">
   <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="61.5703125" customWidth="1"/>
+    <col min="4" max="4" width="61.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
@@ -2679,7 +2682,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -2702,7 +2705,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
@@ -2725,7 +2728,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
         <v>27</v>
@@ -2746,7 +2749,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
         <v>29</v>
@@ -2767,7 +2770,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
         <v>31</v>
@@ -2788,7 +2791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
@@ -2811,7 +2814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>36</v>
@@ -2832,7 +2835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>38</v>
@@ -2853,7 +2856,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6" t="s">
         <v>40</v>
@@ -2874,7 +2877,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="6" t="s">
         <v>42</v>
@@ -2886,7 +2889,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>44</v>
       </c>
@@ -2900,7 +2903,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="6" t="s">
         <v>47</v>
@@ -2912,7 +2915,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6" t="s">
         <v>49</v>
@@ -2924,7 +2927,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="6" t="s">
         <v>51</v>
@@ -2936,7 +2939,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="6" t="s">
         <v>53</v>
@@ -2948,7 +2951,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6" t="s">
         <v>55</v>
@@ -2960,7 +2963,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>57</v>
       </c>
@@ -2974,7 +2977,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="6" t="s">
         <v>60</v>
@@ -2986,7 +2989,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="6" t="s">
         <v>62</v>
@@ -2998,7 +3001,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="6" t="s">
         <v>64</v>
@@ -3010,7 +3013,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="6" t="s">
         <v>66</v>
@@ -3022,7 +3025,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="B26" s="6" t="s">
         <v>68</v>
@@ -3034,7 +3037,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>70</v>
       </c>
@@ -3048,7 +3051,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="6" t="s">
         <v>73</v>
@@ -3060,7 +3063,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="6" t="s">
         <v>75</v>
@@ -3072,7 +3075,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="6" t="s">
         <v>77</v>
@@ -3084,7 +3087,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="6" t="s">
         <v>79</v>
@@ -3096,7 +3099,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="6" t="s">
         <v>81</v>
@@ -3108,17 +3111,17 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>20</v>
       </c>
@@ -3132,7 +3135,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>85</v>
       </c>
@@ -3146,7 +3149,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
       <c r="B42" s="6" t="s">
         <v>88</v>
@@ -3158,7 +3161,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="6" t="s">
         <v>90</v>
@@ -3170,7 +3173,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>92</v>
       </c>
@@ -3184,7 +3187,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="6" t="s">
         <v>95</v>
@@ -3196,7 +3199,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
       <c r="B46" s="6" t="s">
         <v>97</v>
@@ -3208,7 +3211,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>99</v>
       </c>
@@ -3222,7 +3225,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
       <c r="B48" s="6" t="s">
         <v>102</v>
@@ -3234,7 +3237,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="6" t="s">
         <v>104</v>
@@ -3246,7 +3249,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>106</v>
       </c>
@@ -3260,7 +3263,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
       <c r="B51" s="6" t="s">
         <v>109</v>
@@ -3272,7 +3275,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="6"/>
       <c r="B52" s="6" t="s">
         <v>111</v>
@@ -3284,17 +3287,17 @@
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>20</v>
       </c>
@@ -3308,7 +3311,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
         <v>115</v>
       </c>
@@ -3322,7 +3325,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="6"/>
       <c r="B62" s="6" t="s">
         <v>118</v>
@@ -3334,7 +3337,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="6"/>
       <c r="B63" s="6" t="s">
         <v>120</v>
@@ -3346,7 +3349,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
         <v>122</v>
       </c>
@@ -3360,7 +3363,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="6"/>
       <c r="B65" s="6" t="s">
         <v>125</v>
@@ -3372,7 +3375,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="6"/>
       <c r="B66" s="6" t="s">
         <v>127</v>
@@ -3384,7 +3387,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="6"/>
       <c r="B67" s="6" t="s">
         <v>129</v>
@@ -3396,7 +3399,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
         <v>131</v>
       </c>
@@ -3410,7 +3413,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="6"/>
       <c r="B69" s="6" t="s">
         <v>134</v>
@@ -3422,7 +3425,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="6"/>
       <c r="B70" s="6" t="s">
         <v>136</v>
@@ -3434,7 +3437,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
         <v>138</v>
       </c>
@@ -3448,7 +3451,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="6"/>
       <c r="B72" s="6" t="s">
         <v>141</v>
@@ -3460,7 +3463,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="6"/>
       <c r="B73" s="6" t="s">
         <v>143</v>
@@ -3472,7 +3475,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
         <v>145</v>
       </c>
@@ -3486,7 +3489,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="6"/>
       <c r="B75" s="6" t="s">
         <v>148</v>
@@ -3498,7 +3501,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="6"/>
       <c r="B76" s="6" t="s">
         <v>150</v>
@@ -3510,17 +3513,17 @@
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>20</v>
       </c>
@@ -3534,7 +3537,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
         <v>154</v>
       </c>
@@ -3548,7 +3551,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="6"/>
       <c r="B86" s="6" t="s">
         <v>157</v>
@@ -3560,7 +3563,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="6"/>
       <c r="B87" s="6" t="s">
         <v>159</v>
@@ -3572,7 +3575,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
         <v>161</v>
       </c>
@@ -3586,7 +3589,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="6"/>
       <c r="B89" s="6" t="s">
         <v>164</v>
@@ -3598,7 +3601,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="6"/>
       <c r="B90" s="6" t="s">
         <v>166</v>
@@ -3610,7 +3613,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="8" t="s">
         <v>168</v>
       </c>
@@ -3624,7 +3627,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="6"/>
       <c r="B92" s="6" t="s">
         <v>171</v>
@@ -3636,7 +3639,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
         <v>173</v>
       </c>
@@ -3650,7 +3653,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="6"/>
       <c r="B94" s="6" t="s">
         <v>176</v>
@@ -3662,17 +3665,17 @@
         <v>177</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>20</v>
       </c>
@@ -3686,7 +3689,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="8" t="s">
         <v>180</v>
       </c>
@@ -3700,7 +3703,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="6"/>
       <c r="B104" s="6" t="s">
         <v>183</v>
@@ -3712,7 +3715,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="6"/>
       <c r="B105" s="6" t="s">
         <v>185</v>
@@ -3724,7 +3727,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="8" t="s">
         <v>187</v>
       </c>
@@ -3738,7 +3741,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="6"/>
       <c r="B107" s="6" t="s">
         <v>190</v>
@@ -3750,7 +3753,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="6"/>
       <c r="B108" s="6" t="s">
         <v>192</v>
@@ -3762,7 +3765,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="6"/>
       <c r="B109" s="6" t="s">
         <v>194</v>
@@ -3774,7 +3777,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="8" t="s">
         <v>196</v>
       </c>
@@ -3788,7 +3791,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="6"/>
       <c r="B111" s="6" t="s">
         <v>199</v>
@@ -3800,7 +3803,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="6"/>
       <c r="B112" s="6" t="s">
         <v>201</v>
@@ -3812,7 +3815,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="8" t="s">
         <v>203</v>
       </c>
@@ -3826,7 +3829,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="6"/>
       <c r="B114" s="6" t="s">
         <v>206</v>
@@ -3838,7 +3841,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="6"/>
       <c r="B115" s="6" t="s">
         <v>208</v>
@@ -3850,7 +3853,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="6"/>
       <c r="B116" s="6" t="s">
         <v>210</v>
@@ -3862,17 +3865,17 @@
         <v>211</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
         <v>20</v>
       </c>
@@ -3886,7 +3889,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="8" t="s">
         <v>214</v>
       </c>
@@ -3900,7 +3903,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="6"/>
       <c r="B126" s="6" t="s">
         <v>217</v>
@@ -3912,7 +3915,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="6"/>
       <c r="B127" s="6" t="s">
         <v>219</v>
@@ -3924,7 +3927,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="8" t="s">
         <v>221</v>
       </c>
@@ -3938,7 +3941,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="6"/>
       <c r="B129" s="6" t="s">
         <v>224</v>
@@ -3950,7 +3953,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="6"/>
       <c r="B130" s="6" t="s">
         <v>226</v>
@@ -3962,7 +3965,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="8" t="s">
         <v>228</v>
       </c>
@@ -3976,7 +3979,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="6"/>
       <c r="B132" s="6" t="s">
         <v>231</v>
@@ -3988,7 +3991,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="6"/>
       <c r="B133" s="6" t="s">
         <v>233</v>
@@ -4000,7 +4003,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="8" t="s">
         <v>235</v>
       </c>
@@ -4014,7 +4017,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="6"/>
       <c r="B135" s="6" t="s">
         <v>238</v>
@@ -4026,17 +4029,17 @@
         <v>239</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
         <v>20</v>
       </c>
@@ -4050,7 +4053,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="8" t="s">
         <v>242</v>
       </c>
@@ -4064,7 +4067,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="6"/>
       <c r="B145" s="6" t="s">
         <v>245</v>
@@ -4076,7 +4079,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="6"/>
       <c r="B146" s="6" t="s">
         <v>247</v>
@@ -4088,7 +4091,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="6"/>
       <c r="B147" s="6" t="s">
         <v>249</v>
@@ -4100,7 +4103,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="8" t="s">
         <v>251</v>
       </c>
@@ -4114,7 +4117,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="6"/>
       <c r="B149" s="6" t="s">
         <v>254</v>
@@ -4126,7 +4129,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="6"/>
       <c r="B150" s="6" t="s">
         <v>256</v>
@@ -4138,7 +4141,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="8" t="s">
         <v>258</v>
       </c>
@@ -4152,7 +4155,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="6"/>
       <c r="B152" s="6" t="s">
         <v>261</v>
@@ -4164,7 +4167,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="6"/>
       <c r="B153" s="6" t="s">
         <v>263</v>
@@ -4176,7 +4179,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="8" t="s">
         <v>265</v>
       </c>
@@ -4190,7 +4193,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="6"/>
       <c r="B155" s="6" t="s">
         <v>268</v>
@@ -4202,7 +4205,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="6"/>
       <c r="B156" s="6" t="s">
         <v>270</v>
@@ -4214,7 +4217,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="6"/>
       <c r="B157" s="6" t="s">
         <v>272</v>
@@ -4226,7 +4229,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>274</v>
       </c>
@@ -4240,21 +4243,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD58A5C7-A874-4623-9042-1E94C63ECBF9}">
   <dimension ref="A1:H173"/>
   <sheetViews>
-    <sheetView topLeftCell="A150" workbookViewId="0">
+    <sheetView topLeftCell="A160" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="55.85546875" customWidth="1"/>
+    <col min="4" max="4" width="55.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
@@ -4262,7 +4265,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -4285,7 +4288,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
@@ -4308,7 +4311,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
         <v>27</v>
@@ -4329,7 +4332,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
         <v>29</v>
@@ -4350,7 +4353,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
         <v>31</v>
@@ -4371,7 +4374,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
@@ -4394,7 +4397,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>36</v>
@@ -4415,7 +4418,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>38</v>
@@ -4436,7 +4439,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6" t="s">
         <v>40</v>
@@ -4457,7 +4460,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="6" t="s">
         <v>42</v>
@@ -4469,7 +4472,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>44</v>
       </c>
@@ -4483,7 +4486,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="6" t="s">
         <v>47</v>
@@ -4495,7 +4498,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6" t="s">
         <v>49</v>
@@ -4507,7 +4510,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="6" t="s">
         <v>51</v>
@@ -4519,7 +4522,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="6" t="s">
         <v>53</v>
@@ -4531,7 +4534,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6" t="s">
         <v>55</v>
@@ -4543,7 +4546,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>57</v>
       </c>
@@ -4557,7 +4560,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="6" t="s">
         <v>60</v>
@@ -4569,7 +4572,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="6" t="s">
         <v>62</v>
@@ -4581,7 +4584,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="6" t="s">
         <v>64</v>
@@ -4593,7 +4596,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="6" t="s">
         <v>66</v>
@@ -4605,7 +4608,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="B26" s="6" t="s">
         <v>68</v>
@@ -4617,7 +4620,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>70</v>
       </c>
@@ -4631,7 +4634,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="6" t="s">
         <v>73</v>
@@ -4643,7 +4646,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="6" t="s">
         <v>75</v>
@@ -4655,7 +4658,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="6" t="s">
         <v>77</v>
@@ -4667,7 +4670,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="6" t="s">
         <v>79</v>
@@ -4679,7 +4682,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="6" t="s">
         <v>81</v>
@@ -4691,17 +4694,17 @@
         <v>317</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>20</v>
       </c>
@@ -4715,7 +4718,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>85</v>
       </c>
@@ -4729,7 +4732,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
       <c r="B42" s="6" t="s">
         <v>88</v>
@@ -4741,7 +4744,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="6" t="s">
         <v>90</v>
@@ -4753,7 +4756,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>92</v>
       </c>
@@ -4767,7 +4770,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="6" t="s">
         <v>95</v>
@@ -4779,7 +4782,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
       <c r="B46" s="6" t="s">
         <v>97</v>
@@ -4791,7 +4794,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>99</v>
       </c>
@@ -4805,7 +4808,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
       <c r="B48" s="6" t="s">
         <v>102</v>
@@ -4817,7 +4820,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="6" t="s">
         <v>104</v>
@@ -4829,7 +4832,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>106</v>
       </c>
@@ -4843,7 +4846,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
       <c r="B51" s="6" t="s">
         <v>109</v>
@@ -4855,7 +4858,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="6"/>
       <c r="B52" s="6" t="s">
         <v>111</v>
@@ -4867,17 +4870,17 @@
         <v>330</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>20</v>
       </c>
@@ -4891,7 +4894,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
         <v>115</v>
       </c>
@@ -4905,7 +4908,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="6"/>
       <c r="B62" s="6" t="s">
         <v>118</v>
@@ -4917,7 +4920,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="6"/>
       <c r="B63" s="6" t="s">
         <v>120</v>
@@ -4929,7 +4932,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
         <v>122</v>
       </c>
@@ -4943,7 +4946,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="6"/>
       <c r="B65" s="6" t="s">
         <v>125</v>
@@ -4955,7 +4958,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="6"/>
       <c r="B66" s="6" t="s">
         <v>127</v>
@@ -4967,7 +4970,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="6"/>
       <c r="B67" s="6" t="s">
         <v>129</v>
@@ -4979,7 +4982,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
         <v>131</v>
       </c>
@@ -4993,7 +4996,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="6"/>
       <c r="B69" s="6" t="s">
         <v>134</v>
@@ -5005,7 +5008,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="6"/>
       <c r="B70" s="6" t="s">
         <v>136</v>
@@ -5017,7 +5020,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
         <v>138</v>
       </c>
@@ -5031,7 +5034,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="6"/>
       <c r="B72" s="6" t="s">
         <v>141</v>
@@ -5043,7 +5046,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="6"/>
       <c r="B73" s="6" t="s">
         <v>143</v>
@@ -5055,7 +5058,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
         <v>145</v>
       </c>
@@ -5069,7 +5072,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="6"/>
       <c r="B75" s="6" t="s">
         <v>148</v>
@@ -5081,7 +5084,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="6"/>
       <c r="B76" s="6" t="s">
         <v>150</v>
@@ -5093,17 +5096,17 @@
         <v>347</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>20</v>
       </c>
@@ -5117,7 +5120,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
         <v>154</v>
       </c>
@@ -5131,7 +5134,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="6"/>
       <c r="B86" s="6" t="s">
         <v>157</v>
@@ -5143,7 +5146,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="6"/>
       <c r="B87" s="6" t="s">
         <v>159</v>
@@ -5155,7 +5158,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
         <v>161</v>
       </c>
@@ -5169,7 +5172,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="6"/>
       <c r="B89" s="6" t="s">
         <v>164</v>
@@ -5181,7 +5184,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="6"/>
       <c r="B90" s="6" t="s">
         <v>166</v>
@@ -5193,7 +5196,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="8" t="s">
         <v>168</v>
       </c>
@@ -5207,7 +5210,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="6"/>
       <c r="B92" s="6" t="s">
         <v>171</v>
@@ -5219,7 +5222,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
         <v>173</v>
       </c>
@@ -5233,7 +5236,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="6"/>
       <c r="B94" s="6" t="s">
         <v>176</v>
@@ -5245,17 +5248,17 @@
         <v>358</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>20</v>
       </c>
@@ -5269,7 +5272,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="8" t="s">
         <v>180</v>
       </c>
@@ -5283,7 +5286,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="6"/>
       <c r="B104" s="6" t="s">
         <v>183</v>
@@ -5295,7 +5298,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="6"/>
       <c r="B105" s="6" t="s">
         <v>185</v>
@@ -5307,7 +5310,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="8" t="s">
         <v>187</v>
       </c>
@@ -5321,7 +5324,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="6"/>
       <c r="B107" s="6" t="s">
         <v>190</v>
@@ -5333,7 +5336,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="6"/>
       <c r="B108" s="6" t="s">
         <v>192</v>
@@ -5345,7 +5348,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="6"/>
       <c r="B109" s="6" t="s">
         <v>194</v>
@@ -5357,7 +5360,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="8" t="s">
         <v>196</v>
       </c>
@@ -5371,7 +5374,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="6"/>
       <c r="B111" s="6" t="s">
         <v>199</v>
@@ -5383,7 +5386,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="6"/>
       <c r="B112" s="6" t="s">
         <v>201</v>
@@ -5395,7 +5398,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="8" t="s">
         <v>203</v>
       </c>
@@ -5409,7 +5412,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="6"/>
       <c r="B114" s="6" t="s">
         <v>206</v>
@@ -5421,7 +5424,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="6"/>
       <c r="B115" s="6" t="s">
         <v>208</v>
@@ -5433,7 +5436,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="6"/>
       <c r="B116" s="6" t="s">
         <v>210</v>
@@ -5445,17 +5448,17 @@
         <v>373</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
         <v>20</v>
       </c>
@@ -5469,7 +5472,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="8" t="s">
         <v>214</v>
       </c>
@@ -5483,7 +5486,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="6"/>
       <c r="B126" s="6" t="s">
         <v>217</v>
@@ -5495,7 +5498,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="6"/>
       <c r="B127" s="6" t="s">
         <v>219</v>
@@ -5507,7 +5510,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="8" t="s">
         <v>221</v>
       </c>
@@ -5521,7 +5524,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="6"/>
       <c r="B129" s="6" t="s">
         <v>224</v>
@@ -5533,7 +5536,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="6"/>
       <c r="B130" s="6" t="s">
         <v>226</v>
@@ -5545,7 +5548,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="8" t="s">
         <v>228</v>
       </c>
@@ -5559,7 +5562,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="6"/>
       <c r="B132" s="6" t="s">
         <v>231</v>
@@ -5571,7 +5574,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="6"/>
       <c r="B133" s="6" t="s">
         <v>233</v>
@@ -5583,7 +5586,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="8" t="s">
         <v>235</v>
       </c>
@@ -5597,7 +5600,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="6"/>
       <c r="B135" s="6" t="s">
         <v>238</v>
@@ -5609,17 +5612,17 @@
         <v>385</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
         <v>20</v>
       </c>
@@ -5633,7 +5636,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="8" t="s">
         <v>242</v>
       </c>
@@ -5647,7 +5650,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="6"/>
       <c r="B145" s="6" t="s">
         <v>245</v>
@@ -5659,7 +5662,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="6"/>
       <c r="B146" s="6" t="s">
         <v>247</v>
@@ -5671,7 +5674,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="6"/>
       <c r="B147" s="6" t="s">
         <v>249</v>
@@ -5683,7 +5686,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="8" t="s">
         <v>251</v>
       </c>
@@ -5697,7 +5700,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="6"/>
       <c r="B149" s="6" t="s">
         <v>254</v>
@@ -5709,7 +5712,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="6"/>
       <c r="B150" s="6" t="s">
         <v>256</v>
@@ -5721,7 +5724,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="8" t="s">
         <v>258</v>
       </c>
@@ -5735,7 +5738,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="6"/>
       <c r="B152" s="6" t="s">
         <v>261</v>
@@ -5747,7 +5750,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="6"/>
       <c r="B153" s="6" t="s">
         <v>263</v>
@@ -5759,7 +5762,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="8" t="s">
         <v>265</v>
       </c>
@@ -5773,7 +5776,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="6"/>
       <c r="B155" s="6" t="s">
         <v>268</v>
@@ -5785,7 +5788,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="6"/>
       <c r="B156" s="6" t="s">
         <v>270</v>
@@ -5797,7 +5800,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="6"/>
       <c r="B157" s="6" t="s">
         <v>272</v>
@@ -5809,17 +5812,17 @@
         <v>400</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="24" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" ht="24" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="5" t="s">
         <v>276</v>
       </c>
@@ -5830,7 +5833,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="6" t="s">
         <v>279</v>
       </c>
@@ -5841,7 +5844,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="6" t="s">
         <v>281</v>
       </c>
@@ -5852,7 +5855,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="6" t="s">
         <v>283</v>
       </c>
@@ -5863,7 +5866,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="6" t="s">
         <v>285</v>
       </c>
@@ -5874,7 +5877,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A170" s="6" t="s">
         <v>286</v>
       </c>
@@ -5885,7 +5888,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="6" t="s">
         <v>287</v>
       </c>
@@ -5896,7 +5899,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="6" t="s">
         <v>288</v>
       </c>
@@ -5907,7 +5910,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="8" t="s">
         <v>289</v>
       </c>
@@ -5927,32 +5930,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0016AF89-A296-4EEC-A259-3B685939663E}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="47.5703125" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="47.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>404</v>
       </c>
@@ -5969,7 +5972,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
         <v>34</v>
       </c>
@@ -5986,7 +5989,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>116</v>
       </c>
@@ -6003,7 +6006,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
         <v>132</v>
       </c>
@@ -6020,7 +6023,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
         <v>136</v>
       </c>
@@ -6037,7 +6040,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
         <v>146</v>
       </c>
@@ -6054,7 +6057,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
         <v>127</v>
       </c>
@@ -6071,7 +6074,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
         <v>97</v>
       </c>
@@ -6088,7 +6091,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
         <v>416</v>
       </c>
@@ -6105,12 +6108,12 @@
         <v>417</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="19" x14ac:dyDescent="0.2">
       <c r="B17" s="7" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
         <v>404</v>
       </c>
@@ -6127,7 +6130,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
         <v>51</v>
       </c>
@@ -6144,7 +6147,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
         <v>49</v>
       </c>
@@ -6161,7 +6164,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
         <v>58</v>
       </c>
@@ -6178,7 +6181,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
         <v>60</v>
       </c>
@@ -6195,7 +6198,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>62</v>
       </c>
@@ -6212,7 +6215,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
         <v>66</v>
       </c>
@@ -6229,7 +6232,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
         <v>159</v>
       </c>
@@ -6246,7 +6249,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
         <v>166</v>
       </c>
@@ -6263,25 +6266,24 @@
         <v>426</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="C28" s="9">
-        <v>45752</v>
-      </c>
-      <c r="D28" s="9">
-        <v>45691</v>
+      <c r="C28" s="18">
+        <v>5</v>
+      </c>
+      <c r="D28" s="18">
+        <v>2</v>
       </c>
       <c r="E28" s="6">
-        <f>2-3</f>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
         <v>429</v>
       </c>
@@ -6298,7 +6300,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
         <v>431</v>
       </c>
@@ -6315,7 +6317,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
         <v>433</v>
       </c>
@@ -6332,12 +6334,12 @@
         <v>434</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" ht="19" x14ac:dyDescent="0.2">
       <c r="B33" s="7" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
         <v>404</v>
       </c>
@@ -6351,7 +6353,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" ht="32" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
         <v>45</v>
       </c>
@@ -6365,7 +6367,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" ht="32" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
         <v>71</v>
       </c>
@@ -6379,7 +6381,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" ht="32" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
         <v>55</v>
       </c>
@@ -6393,7 +6395,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B39" s="6" t="s">
         <v>188</v>
       </c>
@@ -6407,15 +6409,15 @@
         <v>440</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" ht="32" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="C40" s="9">
-        <v>45720</v>
-      </c>
-      <c r="D40" s="9">
-        <v>45720</v>
+      <c r="C40" s="19">
+        <v>3</v>
+      </c>
+      <c r="D40" s="19">
+        <v>3</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>442</v>

</xml_diff>